<commit_message>
excel write file existed
</commit_message>
<xml_diff>
--- a/src/Sample.xlsx
+++ b/src/Sample.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yahyakansu/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yahyakansu/IdeaProjects/SampleProject/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B4B6E44-6D94-7C4D-AA27-1245FE5CF179}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A588CC65-C0E5-DE43-9447-9CED2540CF02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{FADD78F1-9901-F04E-95D0-C304A2DE6C43}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" activeTab="1" xr2:uid="{FADD78F1-9901-F04E-95D0-C304A2DE6C43}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -422,8 +423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF34F02D-5F72-A544-95E7-4334B738F26E}">
   <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -469,4 +470,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A7185DB-6220-524C-9079-FF505A72D36B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
products and prices added to the List with TestNG
</commit_message>
<xml_diff>
--- a/src/Sample.xlsx
+++ b/src/Sample.xlsx
@@ -3,22 +3,23 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yahyakansu/IdeaProjects/SampleProject/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A588CC65-C0E5-DE43-9447-9CED2540CF02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070F3FE2-6700-FE45-A0A6-A5AB83211F07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" activeTab="1" xr2:uid="{FADD78F1-9901-F04E-95D0-C304A2DE6C43}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" activeTab="2" xr2:uid="{FADD78F1-9901-F04E-95D0-C304A2DE6C43}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="collection" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -79,7 +80,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -480,11 +480,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A7185DB-6220-524C-9079-FF505A72D36B}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -492,4 +492,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{134F1CF8-9FD2-104E-8086-A26E6AC3556B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
create Lists from website
</commit_message>
<xml_diff>
--- a/src/Sample.xlsx
+++ b/src/Sample.xlsx
@@ -3,23 +3,23 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yahyakansu/IdeaProjects/SampleProject/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070F3FE2-6700-FE45-A0A6-A5AB83211F07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5239DB5-1629-E24E-B884-8BB6486228BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" activeTab="2" xr2:uid="{FADD78F1-9901-F04E-95D0-C304A2DE6C43}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="collection" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>first name</t>
   </si>
@@ -74,12 +74,25 @@
   </si>
   <si>
     <t>Hello World</t>
+  </si>
+  <si>
+    <t>PRODUCTS</t>
+  </si>
+  <si>
+    <t>PRICES</t>
+  </si>
+  <si>
+    <t>PRODUCTSfadfsa</t>
+  </si>
+  <si>
+    <t>PRICESfasdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -495,13 +508,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{134F1CF8-9FD2-104E-8086-A26E6AC3556B}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06A98CAC-ADE0-524A-BACE-1436342AE949}">
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
product and price infos writed to the excel file from website
</commit_message>
<xml_diff>
--- a/src/Sample.xlsx
+++ b/src/Sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yahyakansu/IdeaProjects/SampleProject/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5239DB5-1629-E24E-B884-8BB6486228BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96EDC84-D5ED-7A40-AC3B-0DD412B5AA31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" activeTab="2" xr2:uid="{FADD78F1-9901-F04E-95D0-C304A2DE6C43}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="144">
   <si>
     <t>first name</t>
   </si>
@@ -82,10 +82,474 @@
     <t>PRICES</t>
   </si>
   <si>
-    <t>PRODUCTSfadfsa</t>
-  </si>
-  <si>
-    <t>PRICESfasdf</t>
+    <t>Uenjoy Indoor and Outdoor Toy Swing for 1-3 Years Old Toddlers and Kids, Three Height Adjustable Swing, with Music</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$64.99</t>
+  </si>
+  <si>
+    <t>Uenjoy 12V 2 Seats Mercedes Benz G63 Kids Ride On Car Electric Cars Motorized Vehicles</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$399.99</t>
+  </si>
+  <si>
+    <t>Uenjoy 12V Electric Ride on Cars, Realistic Off-Road UTV, 2 Seats</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$459.99
++</t>
+  </si>
+  <si>
+    <t>Uenjoy 12V Kids Electric 4-Wheeler ATV Quad Ride On Car</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$189.99
++</t>
+  </si>
+  <si>
+    <t>Uenjoy 12V Kids Electric Ride On Car Lamborghini Huracán Motorized Vehicles</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$169.99
++</t>
+  </si>
+  <si>
+    <t>Uenjoy 12V Kids Electric Ride On Car Lamborghini License Motorized Vehicles</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$269.99</t>
+  </si>
+  <si>
+    <t>Uenjoy 12V Kids Electric Ride On Car Lamborghini License with Remote Control</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$169.99</t>
+  </si>
+  <si>
+    <t>Uenjoy 12V Kids Police Ride On Car SUV Battery Operated Electric Cars</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$154.99
++</t>
+  </si>
+  <si>
+    <t>Uenjoy 12V Kids Ride On Car Electric Cars Licensed GMC</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$430.99
++</t>
+  </si>
+  <si>
+    <t>Uenjoy 12V Large Kids Electric Ride on Car 2 Seats Motorized Truck Battery Powered Children Electric Vehicles</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$279.99</t>
+  </si>
+  <si>
+    <t>Uenjoy 12V Licensed Bugatti Chiron Kids Ride On Car Battery Operated</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$209.99
++</t>
+  </si>
+  <si>
+    <t>Uenjoy 12V Licensed Bugatti Divo Kids Ride On Car Electric Cars</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$249.99</t>
+  </si>
+  <si>
+    <t>Uenjoy 12V Licensed Mercedes-Benz G63 Kids Ride On Car Electric Cars</t>
+  </si>
+  <si>
+    <t>SALE PRICE
+$179.99
++</t>
+  </si>
+  <si>
+    <t>Uenjoy 12V Licensed Mercedes-Benz SL500 Kids Ride On Car</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$204.99</t>
+  </si>
+  <si>
+    <t>Uenjoy 2 in 1 Kids Toy Storage Rack with 8 Large Storage Drawers Corner Rack, Suitable for Boys Girls' Bedroom</t>
+  </si>
+  <si>
+    <t>SALE PRICE
+$86.99</t>
+  </si>
+  <si>
+    <t>Uenjoy 2 in 1 Kids Toy Storage Rack with Bookshelf 8 Large Storage Drawers,Suitable for Boys Girls' Bedroom, Living Room, and Kindergarten</t>
+  </si>
+  <si>
+    <t>SALE PRICE
+$88.99</t>
+  </si>
+  <si>
+    <t>Uenjoy 2 in 1 Toddler Slide &amp; Rocking Toy, Lightweight Sturdy Portable Play Slide Climber for Children</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$52.99</t>
+  </si>
+  <si>
+    <t>Uenjoy 2 Seater 12V Licensed Mercedes-Benz GLS63 AMG Kids Ride On Car</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$409.99</t>
+  </si>
+  <si>
+    <t>Uenjoy 2 Seats 12V Electric Kids Ride On Car Mercedes Benz License Toys</t>
+  </si>
+  <si>
+    <t>SALE PRICE
+$389.99
++</t>
+  </si>
+  <si>
+    <t>Uenjoy 2 Seats Kids Car 12V Ride On Racer Cars Battery Operated 3 Colors</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$369.99
++</t>
+  </si>
+  <si>
+    <t>Uenjoy 2 Seats Kids Car 12V Ride On Racer Cars Battery Operated 5 Colors</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$389.99
++</t>
+  </si>
+  <si>
+    <t>Uenjoy 2-in-1 Kick Scooter with Removable Seat Kids 3 Wheel Foldable Scooter</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$44.99</t>
+  </si>
+  <si>
+    <t>Uenjoy 24V Kids ATV 4 Wheeler Ride On Quad Battery Powered</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$194.99
++</t>
+  </si>
+  <si>
+    <t>Uenjoy 3 in 1 Kids Rocking Horse - Sliding Toy with Balancing Board Ride for Kids Ages 2-5 Years Old</t>
+  </si>
+  <si>
+    <t>SALE PRICE
+$53.99</t>
+  </si>
+  <si>
+    <t>Uenjoy 3 in 1 Kids Toy Storage Rack with Bookshelf 8 Large Storage Drawers&amp;Corner Rack</t>
+  </si>
+  <si>
+    <t>SALE PRICE
+$99.99</t>
+  </si>
+  <si>
+    <t>Uenjoy 3-in-1 Kids Basketball Hoop Set Stand Height Adjustable Easy Score Basketball Set Soccer Goal &amp; Golf Game for Toddlers Kids Indoor and Outdoor</t>
+  </si>
+  <si>
+    <t>SALE PRICE
+$52.99</t>
+  </si>
+  <si>
+    <t>Uenjoy 4-in-1 Slide and Swing Set for Toddlers, Play Climber</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$309.99</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$274.99</t>
+  </si>
+  <si>
+    <t>Uenjoy 5 in 1 Baby High Chair Dining Chair, Rocking Chair, Walker</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$99.99
++</t>
+  </si>
+  <si>
+    <t>Uenjoy 6-in-1 Kick Scooter Kids Balance Bike Tricycle with Detachable Push Handle</t>
+  </si>
+  <si>
+    <t>SALE PRICE
+$69.99</t>
+  </si>
+  <si>
+    <t>Uenjoy 6V Kids/Toddler/Babies Police Ride On Toy Battery Operated Electric Cars for Boys&amp;Girls</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$88.99
++</t>
+  </si>
+  <si>
+    <t>Uenjoy 6V Push Ride on Car 3 in 1 Convertible Baby Toddler Stroller</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$69.99</t>
+  </si>
+  <si>
+    <t>Uenjoy Adjustable Hoverboard Seat Attachment Go Kart Accessories</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$79.99</t>
+  </si>
+  <si>
+    <t>Uenjoy Baby Balance Bike 1 Year Old Boys Girls Bicycle Riding Toys and Walker</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$41.99</t>
+  </si>
+  <si>
+    <t>Uenjoy Baby Bassinet, Bedside Sleeper,Baby Bed to Bed, Adjustable Portable Bed for Infant/Baby Boy &amp; Girl/Newborn,with Mosquito nets</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$99.99</t>
+  </si>
+  <si>
+    <t>Uenjoy Baby Climber Slide Toddler Indoor and Outdoor Freestanding Slide Playset Baby Playground with Basketball Hoop</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$50.99
++</t>
+  </si>
+  <si>
+    <t>Uenjoy Baby Double Seat Jogging Stroller Fold Stroller for Babies &amp; Toddlers with Spring Damping&amp; Lockable Universal Wheels</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$109.99</t>
+  </si>
+  <si>
+    <t>Uenjoy Baby High Chair Dining Chair, One-Click Folding, with Safety Belt</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$66.99
++</t>
+  </si>
+  <si>
+    <t>Uenjoy Baby High Chair with Soft Seat Cushion, Adjustable Seat Belt</t>
+  </si>
+  <si>
+    <t>Uenjoy Baby Lightweight Jogging Stroller One-Click Folding Stroller</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$89.99</t>
+  </si>
+  <si>
+    <t>Uenjoy Baby Playpen 12 Panel Adjustable Kids Safety Activity Center Play</t>
+  </si>
+  <si>
+    <t>Uenjoy Baby Playpen 14 Panel Baby Fence One-Click Folding Playground for Babies &amp;Toddlers Adjustable Safety Activity</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$109.99
++</t>
+  </si>
+  <si>
+    <t>Uenjoy Children's Color Game Fence, Baby Crawling Safety Fence</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$119.99</t>
+  </si>
+  <si>
+    <t>Uenjoy Children's Electric Car Mercedes-Benz Maybach Ride On Car</t>
+  </si>
+  <si>
+    <t>SALE PRICE
+$209.99
++</t>
+  </si>
+  <si>
+    <t>Uenjoy Children's Safety Playpen, Baby Crawling Mat</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$115.99</t>
+  </si>
+  <si>
+    <t>Uenjoy Electric Kids Ride On Car Mercedes Benz AMG GTR License</t>
+  </si>
+  <si>
+    <t>SALE PRICE
+$169.99
++</t>
+  </si>
+  <si>
+    <t>Uenjoy Electric Kids Ride On Cars Battery Motorized Vehicles with Remote Control</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$139.99</t>
+  </si>
+  <si>
+    <t>Uenjoy Electric Kids Ride On Cars Truck 12V Battery Power Vehicles Remote Control</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$219.99
++</t>
+  </si>
+  <si>
+    <t>Uenjoy Electric Ride On Tractor with Trailer, Electric Tractor Motorized Vehicles</t>
+  </si>
+  <si>
+    <t>Uenjoy Kart On Foot Ride On Car, Large Riding Toys</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$149.99</t>
+  </si>
+  <si>
+    <t>Uenjoy Kick Scooter Kids 3 Wheel Scooter, Adjustable Height</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$39.99</t>
+  </si>
+  <si>
+    <t>Uenjoy Kids Balance Bike No Pedal Bicycle for 2-4 Years Old</t>
+  </si>
+  <si>
+    <t>Uenjoy Kids Balance Bike No Pedal Bicycle Red 3</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$34.99</t>
+  </si>
+  <si>
+    <t>Uenjoy Kids Book Rack Storage Child Bookshelf, Four-Frame Kids Bookshelf,Boys and Girls Room Decoration Bookshelf</t>
+  </si>
+  <si>
+    <t>SALE PRICE
+$51.99</t>
+  </si>
+  <si>
+    <t>Uenjoy Kids Climber Indoor and Outdoor Freestanding Slide Playset</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$54.99</t>
+  </si>
+  <si>
+    <t>Uenjoy Kids Climber Slide Toddler, Freestanding Slide Playset</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$84.99</t>
+  </si>
+  <si>
+    <t>Uenjoy Kids Electric Ride on Cars 6v Battery Power Motorized Vehicles</t>
+  </si>
+  <si>
+    <t>Uenjoy Kids Mini Kitchen Playset Plastic Pretend Play Kitchen with Realistic Lights &amp; Sounds</t>
+  </si>
+  <si>
+    <t>SALE PRICE
+$49.99</t>
+  </si>
+  <si>
+    <t>SALE PRICE
+$54.99</t>
+  </si>
+  <si>
+    <t>Uenjoy Kids Mini Kitchen Playset Plastic Pretend Play Kitchen with Realistic Lights &amp; Sounds, Kitchen Sink with Real Water</t>
+  </si>
+  <si>
+    <t>SALE PRICE
+$44.99</t>
+  </si>
+  <si>
+    <t>Uenjoy Kids Mini Kitchen Playset Plastic Pretend Play Kitchen with Realistic Lights &amp; Sounds, Spray Function &amp; Kitchen Sink</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$62.99</t>
+  </si>
+  <si>
+    <t>Uenjoy Kids Ride On Car 12V Licensed Benz EQC Electric Car</t>
+  </si>
+  <si>
+    <t>Uenjoy Kids Ride On Motorcycle 6V Electric Battery Powered Motorbike for Kids</t>
+  </si>
+  <si>
+    <t>Uenjoy Kids Ride on Unicorn Riding Horse Toy, Pony Rider Mechanical Cycle Walking Action Plush Animal for Children 4 to 9 Years</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$199.99</t>
+  </si>
+  <si>
+    <t>Uenjoy Kids Swing Scooter 3 Wheels Foldable Swing Car</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$61.99
++</t>
+  </si>
+  <si>
+    <t>Uenjoy Kids Toy Storage Rack with 8 Large Storage Drawers,Suitable for Boys Girls' Bedroom, Living Room, and Kindergarten</t>
+  </si>
+  <si>
+    <t>SALE PRICE
+$65.99</t>
+  </si>
+  <si>
+    <t>Uenjoy Kids' Go Kart,Kart On Foot,Pedal Kart,Riding Toys for Boys and Girls Aged 3-8,Outdoor Games and Outdoor Toys</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$79.99
++</t>
+  </si>
+  <si>
+    <t>Uenjoy Licensed Audi A3 12V Kids Ride On Car Electric Cars</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$170.99</t>
+  </si>
+  <si>
+    <t>Uenjoy Licensed Maserati GranCabrio 12V Electric Kids Ride On Cars</t>
+  </si>
+  <si>
+    <t>REGULAR PRICE
+$209.99</t>
   </si>
 </sst>
 </file>
@@ -122,8 +586,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,18 +976,599 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06A98CAC-ADE0-524A-BACE-1436342AE949}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.83203125" collapsed="false"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>78</v>
+      </c>
+      <c r="B34" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>86</v>
+      </c>
+      <c r="B38" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>88</v>
+      </c>
+      <c r="B39" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>90</v>
+      </c>
+      <c r="B40" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>91</v>
+      </c>
+      <c r="B41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>93</v>
+      </c>
+      <c r="B42" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>94</v>
+      </c>
+      <c r="B43" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>96</v>
+      </c>
+      <c r="B44" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>98</v>
+      </c>
+      <c r="B45" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>100</v>
+      </c>
+      <c r="B46" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>102</v>
+      </c>
+      <c r="B47" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>104</v>
+      </c>
+      <c r="B48" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>106</v>
+      </c>
+      <c r="B49" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>108</v>
+      </c>
+      <c r="B50" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>109</v>
+      </c>
+      <c r="B51" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>111</v>
+      </c>
+      <c r="B52" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>113</v>
+      </c>
+      <c r="B53" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>113</v>
+      </c>
+      <c r="B54" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>114</v>
+      </c>
+      <c r="B55" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>116</v>
+      </c>
+      <c r="B56" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>118</v>
+      </c>
+      <c r="B57" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>120</v>
+      </c>
+      <c r="B58" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>122</v>
+      </c>
+      <c r="B59" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>123</v>
+      </c>
+      <c r="B60" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>123</v>
+      </c>
+      <c r="B61" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>123</v>
+      </c>
+      <c r="B62" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>123</v>
+      </c>
+      <c r="B63" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>126</v>
+      </c>
+      <c r="B64" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>128</v>
+      </c>
+      <c r="B65" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>130</v>
+      </c>
+      <c r="B66" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>131</v>
+      </c>
+      <c r="B67" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>132</v>
+      </c>
+      <c r="B68" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>134</v>
+      </c>
+      <c r="B69" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>136</v>
+      </c>
+      <c r="B70" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>138</v>
+      </c>
+      <c r="B71" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>140</v>
+      </c>
+      <c r="B72" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>142</v>
+      </c>
+      <c r="B73" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created test that data transfer from MySQL to the Excel
</commit_message>
<xml_diff>
--- a/src/Sample.xlsx
+++ b/src/Sample.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yahyakansu/IdeaProjects/SampleProject/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09709D79-336E-C547-8883-77B4AF43FA37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA262D0-9BAF-CD40-A73A-3AC68CAD4085}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" activeTab="2" xr2:uid="{FADD78F1-9901-F04E-95D0-C304A2DE6C43}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" activeTab="3" xr2:uid="{FADD78F1-9901-F04E-95D0-C304A2DE6C43}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="208">
   <si>
     <t>first name</t>
   </si>
@@ -590,6 +591,162 @@
   <si>
     <t>REGULAR PRICE
 $224.99</t>
+  </si>
+  <si>
+    <t>COUNTY_ID</t>
+  </si>
+  <si>
+    <t>COUNTY_NAME</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>AU</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>BR</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>CH</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>CN</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>DK</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>EG</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>FR</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>HK</t>
+  </si>
+  <si>
+    <t>HongKong</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>Israel</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>JP</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>KW</t>
+  </si>
+  <si>
+    <t>Kuwait</t>
+  </si>
+  <si>
+    <t>MX</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>NG</t>
+  </si>
+  <si>
+    <t>Nigeria</t>
+  </si>
+  <si>
+    <t>NL</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>SG</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>United States of America</t>
+  </si>
+  <si>
+    <t>ZM</t>
+  </si>
+  <si>
+    <t>Zambia</t>
+  </si>
+  <si>
+    <t>ZW</t>
+  </si>
+  <si>
+    <t>Zimbabwe</t>
   </si>
 </sst>
 </file>
@@ -1015,661 +1172,884 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06A98CAC-ADE0-524A-BACE-1436342AE949}">
   <dimension ref="A1:B81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="22.83203125" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.83203125" collapsed="true"/>
   </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>79</v>
+      </c>
+      <c r="B35" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>83</v>
+      </c>
+      <c r="B37" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>85</v>
+      </c>
+      <c r="B38" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>87</v>
+      </c>
+      <c r="B39" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>89</v>
+      </c>
+      <c r="B40" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B41" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>92</v>
+      </c>
+      <c r="B42" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>93</v>
+      </c>
+      <c r="B43" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>95</v>
+      </c>
+      <c r="B44" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>97</v>
+      </c>
+      <c r="B45" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>99</v>
+      </c>
+      <c r="B46" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>101</v>
+      </c>
+      <c r="B47" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>103</v>
+      </c>
+      <c r="B48" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>105</v>
+      </c>
+      <c r="B49" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>107</v>
+      </c>
+      <c r="B50" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>108</v>
+      </c>
+      <c r="B51" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>110</v>
+      </c>
+      <c r="B52" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>112</v>
+      </c>
+      <c r="B53" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>112</v>
+      </c>
+      <c r="B54" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>113</v>
+      </c>
+      <c r="B55" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>115</v>
+      </c>
+      <c r="B56" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>117</v>
+      </c>
+      <c r="B57" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>119</v>
+      </c>
+      <c r="B58" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>121</v>
+      </c>
+      <c r="B59" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>122</v>
+      </c>
+      <c r="B60" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>122</v>
+      </c>
+      <c r="B61" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>122</v>
+      </c>
+      <c r="B62" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>122</v>
+      </c>
+      <c r="B63" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>125</v>
+      </c>
+      <c r="B64" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>127</v>
+      </c>
+      <c r="B65" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>129</v>
+      </c>
+      <c r="B66" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>130</v>
+      </c>
+      <c r="B67" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>131</v>
+      </c>
+      <c r="B68" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>133</v>
+      </c>
+      <c r="B69" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>135</v>
+      </c>
+      <c r="B70" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>137</v>
+      </c>
+      <c r="B71" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>139</v>
+      </c>
+      <c r="B72" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>141</v>
+      </c>
+      <c r="B73" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>143</v>
+      </c>
+      <c r="B74" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>145</v>
+      </c>
+      <c r="B75" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>146</v>
+      </c>
+      <c r="B76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>147</v>
+      </c>
+      <c r="B77" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>148</v>
+      </c>
+      <c r="B78" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>150</v>
+      </c>
+      <c r="B79" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>152</v>
+      </c>
+      <c r="B80" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>154</v>
+      </c>
+      <c r="B81" t="s">
+        <v>155</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05E304F7-0519-0C4A-A453-9823F09EE862}">
+  <dimension ref="A1:B26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>156</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>158</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>162</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>164</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>166</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>168</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>170</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>172</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>174</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>176</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>178</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>180</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>181</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>182</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>184</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>186</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>187</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>188</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>189</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>190</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>192</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
+        <v>193</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>194</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>195</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>52</v>
+        <v>196</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>197</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>54</v>
+        <v>198</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>199</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>56</v>
+        <v>200</v>
       </c>
       <c r="B23" t="s">
-        <v>57</v>
+        <v>201</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>58</v>
+        <v>202</v>
       </c>
       <c r="B24" t="s">
-        <v>59</v>
+        <v>203</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>60</v>
+        <v>204</v>
       </c>
       <c r="B25" t="s">
-        <v>61</v>
+        <v>205</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>62</v>
+        <v>206</v>
       </c>
       <c r="B26" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s">
-        <v>64</v>
-      </c>
-      <c r="B27" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s">
-        <v>66</v>
-      </c>
-      <c r="B28" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s">
-        <v>66</v>
-      </c>
-      <c r="B29" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s">
-        <v>69</v>
-      </c>
-      <c r="B30" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="s">
-        <v>71</v>
-      </c>
-      <c r="B31" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s">
-        <v>73</v>
-      </c>
-      <c r="B32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s">
-        <v>75</v>
-      </c>
-      <c r="B33" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="s">
-        <v>77</v>
-      </c>
-      <c r="B34" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="s">
-        <v>79</v>
-      </c>
-      <c r="B35" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="s">
-        <v>81</v>
-      </c>
-      <c r="B36" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="s">
-        <v>83</v>
-      </c>
-      <c r="B37" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="s">
-        <v>85</v>
-      </c>
-      <c r="B38" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="s">
-        <v>87</v>
-      </c>
-      <c r="B39" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="s">
-        <v>89</v>
-      </c>
-      <c r="B40" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="s">
-        <v>90</v>
-      </c>
-      <c r="B41" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="s">
-        <v>92</v>
-      </c>
-      <c r="B42" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="s">
-        <v>93</v>
-      </c>
-      <c r="B43" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="s">
-        <v>95</v>
-      </c>
-      <c r="B44" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="s">
-        <v>97</v>
-      </c>
-      <c r="B45" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="s">
-        <v>99</v>
-      </c>
-      <c r="B46" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="s">
-        <v>101</v>
-      </c>
-      <c r="B47" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="s">
-        <v>103</v>
-      </c>
-      <c r="B48" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="s">
-        <v>105</v>
-      </c>
-      <c r="B49" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="s">
-        <v>107</v>
-      </c>
-      <c r="B50" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="s">
-        <v>108</v>
-      </c>
-      <c r="B51" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="s">
-        <v>110</v>
-      </c>
-      <c r="B52" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="s">
-        <v>112</v>
-      </c>
-      <c r="B53" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="s">
-        <v>112</v>
-      </c>
-      <c r="B54" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="s">
-        <v>113</v>
-      </c>
-      <c r="B55" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="s">
-        <v>115</v>
-      </c>
-      <c r="B56" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="s">
-        <v>117</v>
-      </c>
-      <c r="B57" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="s">
-        <v>119</v>
-      </c>
-      <c r="B58" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="s">
-        <v>121</v>
-      </c>
-      <c r="B59" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="s">
-        <v>122</v>
-      </c>
-      <c r="B60" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="s">
-        <v>122</v>
-      </c>
-      <c r="B61" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="s">
-        <v>122</v>
-      </c>
-      <c r="B62" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="s">
-        <v>122</v>
-      </c>
-      <c r="B63" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="s">
-        <v>125</v>
-      </c>
-      <c r="B64" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="s">
-        <v>127</v>
-      </c>
-      <c r="B65" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="s">
-        <v>129</v>
-      </c>
-      <c r="B66" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="s">
-        <v>130</v>
-      </c>
-      <c r="B67" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="s">
-        <v>131</v>
-      </c>
-      <c r="B68" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="s">
-        <v>133</v>
-      </c>
-      <c r="B69" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="s">
-        <v>135</v>
-      </c>
-      <c r="B70" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="s">
-        <v>137</v>
-      </c>
-      <c r="B71" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="s">
-        <v>139</v>
-      </c>
-      <c r="B72" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="s">
-        <v>141</v>
-      </c>
-      <c r="B73" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="s">
-        <v>143</v>
-      </c>
-      <c r="B74" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="s">
-        <v>145</v>
-      </c>
-      <c r="B75" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="s">
-        <v>146</v>
-      </c>
-      <c r="B76" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="s">
-        <v>147</v>
-      </c>
-      <c r="B77" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="s">
-        <v>148</v>
-      </c>
-      <c r="B78" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="s">
-        <v>150</v>
-      </c>
-      <c r="B79" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="s">
-        <v>152</v>
-      </c>
-      <c r="B80" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="s">
-        <v>154</v>
-      </c>
-      <c r="B81" t="s">
-        <v>155</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>